<commit_message>
latest code push of Capstone project by Palaniraj
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Guvi Capstone Project.xlsx
+++ b/TestCases/Test Cases Guvi Capstone Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d571de60046687c9/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EclipseWorkspaces\GuviFinalProjects\guviCapstoneProject\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="8_{85EE4C3B-AF60-4858-B626-FC3B1471DE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48BC00E3-8803-4A1B-933F-5E8569108382}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BED75E-446D-4FFC-80FA-C9DD004A0488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
   <si>
     <t>TC_001</t>
   </si>
@@ -124,9 +124,6 @@
     <t>TC_011</t>
   </si>
   <si>
-    <t>Booking Itinerary page should be displayed</t>
-  </si>
-  <si>
     <t>TS_006</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">Selected hotel should be cancelled </t>
-  </si>
-  <si>
-    <t>TC_015</t>
   </si>
   <si>
     <t>1. Application should be stable.                                    
@@ -303,13 +297,6 @@
 Step 2: Enter the "Username"
 Step 3: Enter the "Password"
 Step 4: Click on the "Login" button                                                             
-Step 5: Click on the "Booking Itinerary" link in the search hotel page                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 1: Launch the browser and load the URL "https://adactinhotelapp.com/index.php"
-Step 2: Enter the "Username"
-Step 3: Enter the "Password"
-Step 4: Click on the "Login" button                                                             
 Step 5: Click on the "Booking Itinerary" link in the search hotel page  
 Step 6:  Click on the "Search hotel" button                                                                                                                                                                                                      </t>
   </si>
@@ -388,9 +375,6 @@
 Step 5: Book any hotel and Click on the "Booking Itinerary" link in the search hotel page    
 Step 6: Click on the "Cancel Selected " button                                         
 Step 7: Click on the "Ok" on the alert window                                                                                                                                                                                           </t>
-  </si>
-  <si>
-    <t>Verify user is able to view the booking details without booking</t>
   </si>
   <si>
     <t>Verify user is able to cancel the booked hotel</t>
@@ -820,62 +804,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,10 +876,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1185,9 +1165,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1225,16 +1205,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1242,7 +1222,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>20</v>
@@ -1254,27 +1234,27 @@
         <v>22</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="35" t="s">
-        <v>61</v>
+      <c r="B3" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>20</v>
@@ -1283,27 +1263,27 @@
         <v>5</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1311,27 +1291,27 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1339,22 +1319,22 @@
         <v>7</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="231" thickBot="1" x14ac:dyDescent="0.35">
@@ -1362,7 +1342,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>20</v>
@@ -1371,30 +1351,30 @@
         <v>9</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="346.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>69</v>
+      <c r="B7" s="37" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>20</v>
@@ -1403,27 +1383,27 @@
         <v>10</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="360" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1431,183 +1411,183 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="44"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="44"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="32"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="44"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="44"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="44"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="44"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="45"/>
+    </row>
+    <row r="18" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="29"/>
-    </row>
-    <row r="18" spans="1:10" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
-      <c r="B19" s="46"/>
+      <c r="H18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="41"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1615,182 +1595,146 @@
         <v>30</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="42"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J19" s="16" t="s">
+      <c r="F21" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="33"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="2" t="s">
+      <c r="H21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="360.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="29"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J20" s="16" t="s">
+      <c r="G23" s="13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="34"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="38" t="s">
+      <c r="H23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="360.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="J23" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A7:A17"/>
-    <mergeCell ref="C9:C17"/>
-    <mergeCell ref="D9:D17"/>
-    <mergeCell ref="B7:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
     <mergeCell ref="J9:J17"/>
     <mergeCell ref="G9:G17"/>
     <mergeCell ref="A3:A5"/>
@@ -1799,6 +1743,14 @@
     <mergeCell ref="F9:F17"/>
     <mergeCell ref="H9:H17"/>
     <mergeCell ref="E9:E17"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A7:A17"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="D9:D17"/>
+    <mergeCell ref="B7:B17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>